<commit_message>
Minor tweaks for manuscript version
</commit_message>
<xml_diff>
--- a/Dorey_script/Stats_output.xlsx
+++ b/Dorey_script/Stats_output.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesdorey/Desktop/Uni/My_papers/Elisha_Hons_paper/Honours/Dorey_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A72615-A922-A148-A9FA-BF7A8F7F1133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C454A38D-4EB0-E54A-84B0-4629F980BDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="1000" windowWidth="25020" windowHeight="17440" activeTab="1" xr2:uid="{93F7876E-F456-FA42-A11A-9A49C3A63864}"/>
+    <workbookView xWindow="23180" yWindow="500" windowWidth="25020" windowHeight="17440" activeTab="4" xr2:uid="{93F7876E-F456-FA42-A11A-9A49C3A63864}"/>
   </bookViews>
   <sheets>
     <sheet name="shapiro.test" sheetId="1" r:id="rId1"/>
-    <sheet name="Rfit" sheetId="2" r:id="rId2"/>
+    <sheet name="Rfit_indices" sheetId="2" r:id="rId2"/>
+    <sheet name="Rfit_InfectionDivers" sheetId="4" r:id="rId3"/>
+    <sheet name="Rfit_DiversityRichness" sheetId="5" r:id="rId4"/>
+    <sheet name="Rfit_area" sheetId="6" r:id="rId5"/>
+    <sheet name="SpeciesValues" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="83">
   <si>
     <t>name</t>
   </si>
@@ -150,12 +154,175 @@
   <si>
     <t>.</t>
   </si>
+  <si>
+    <t>Species_name</t>
+  </si>
+  <si>
+    <t>ChaoEstimate</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) achrostus</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) atritergus</t>
+  </si>
+  <si>
+    <t>Infected</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) concavus</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) fijiensis</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) groomi</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) hadrander</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) kaicolo</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) nadarivatu</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) ostridorsum</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. D</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. F</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. G</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. H</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. I</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. J</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. K</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. N</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. O</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. S</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. T</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. U</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. V</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. W</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) sp. X</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) taveuni</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) terminalis</t>
+  </si>
+  <si>
+    <t>Lasioglossum (Homalictus) tuiwawae</t>
+  </si>
+  <si>
+    <t>Sequence count</t>
+  </si>
+  <si>
+    <t>Haplotype count</t>
+  </si>
+  <si>
+    <t>Infection staus</t>
+  </si>
+  <si>
+    <t>Chao estimate</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>&gt; summary(infection_lm)</t>
+  </si>
+  <si>
+    <t>Call:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rfit.default(formula = percentInfected ~ sampleSize + ChaoEstimate, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    data = WolTested_3)</t>
+  </si>
+  <si>
+    <t>Coefficients:</t>
+  </si>
+  <si>
+    <t>sampleSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> t.value</t>
+  </si>
+  <si>
+    <t>summary(infectionDiv_lm)</t>
+  </si>
+  <si>
+    <t>rfit.default(formula = percentInfected ~ Zahl + ChaoEstimate, 
+    data = WolTested_3)</t>
+  </si>
+  <si>
+    <t>n ≥ 3</t>
+  </si>
+  <si>
+    <t>n ≥ 0</t>
+  </si>
+  <si>
+    <t>rfit.default(formula = Zahl ~ ChaoEstimate + WolbachiaDetected, 
+    data = DivRich)</t>
+  </si>
+  <si>
+    <t>rfit.default(formula = percentInfected ~ ChaoEstimate + Zahl + 
+    polygonArea_m2, data = areaPlus)</t>
+  </si>
+  <si>
+    <t>polygonArea_m2</t>
+  </si>
+  <si>
+    <t>summary(areaInfRate_lm)</t>
+  </si>
+  <si>
+    <t>summary(areaDivRich_lm)</t>
+  </si>
+  <si>
+    <t>rfit.default(formula = polygonArea_m2 ~ ChaoEstimate + Zahl + 
+    WolbachiaDetected, data = areaPlus)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -201,6 +368,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFB0B0B0"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -228,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -245,6 +439,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +765,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -793,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B19BD8F-AFC2-804C-9CD6-4FB069BC02A4}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,7 +1487,7 @@
       <c r="C39" s="2">
         <v>2.2118200000000001E-2</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="14">
         <v>8.9488000000000003</v>
       </c>
       <c r="E39" s="3">
@@ -1304,7 +1507,7 @@
       <c r="C40" s="2">
         <v>2.9221E-3</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="14">
         <v>-7.9832999999999998</v>
       </c>
       <c r="E40" s="3">
@@ -1626,4 +1829,1658 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB8E7AC-9CE0-A64E-9EA6-88D096A2F440}">
+  <dimension ref="A1:F68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1.1738999999999999E-2</v>
+      </c>
+      <c r="C10">
+        <v>9.0441099999999999</v>
+      </c>
+      <c r="D10">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E10">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11">
+        <v>-1.9087E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.22679299999999999</v>
+      </c>
+      <c r="D11">
+        <v>-8.4199999999999997E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.93430000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>8.0022999999999997E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.69292900000000002</v>
+      </c>
+      <c r="D12">
+        <v>0.11550000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>1.7987070000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>0.1099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>0.89681999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>-0.96266149999999995</v>
+      </c>
+      <c r="C27">
+        <v>11.867066400000001</v>
+      </c>
+      <c r="D27">
+        <v>-8.1100000000000005E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.93669999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>1.3540272</v>
+      </c>
+      <c r="C28">
+        <v>7.9971975999999998</v>
+      </c>
+      <c r="D28">
+        <v>0.16930000000000001</v>
+      </c>
+      <c r="E28">
+        <v>0.86839999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>5.7019000000000002E-3</v>
+      </c>
+      <c r="C29">
+        <v>0.1354292</v>
+      </c>
+      <c r="D29">
+        <v>4.2099999999999999E-2</v>
+      </c>
+      <c r="E29">
+        <v>0.96709999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <v>4.0236130000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>0.25153999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <v>0.78159999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>5.5413030000000001</v>
+      </c>
+      <c r="C45">
+        <v>21.843284000000001</v>
+      </c>
+      <c r="D45">
+        <v>0.25369999999999998</v>
+      </c>
+      <c r="E45">
+        <v>0.80610000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46">
+        <v>-3.4685000000000001E-2</v>
+      </c>
+      <c r="C46">
+        <v>0.39092399999999999</v>
+      </c>
+      <c r="D46">
+        <v>-8.8700000000000001E-2</v>
+      </c>
+      <c r="E46">
+        <v>0.93149999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47">
+        <v>9.7746E-2</v>
+      </c>
+      <c r="C47">
+        <v>1.2021869999999999</v>
+      </c>
+      <c r="D47">
+        <v>8.1299999999999997E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.93720000000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49">
+        <v>6.3960479999999997E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50">
+        <v>2.5749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>0.97465999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62">
+        <v>0.30317</v>
+      </c>
+      <c r="C62">
+        <v>24.484580000000001</v>
+      </c>
+      <c r="D62">
+        <v>1.24E-2</v>
+      </c>
+      <c r="E62">
+        <v>0.99039999999999995</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>9.6015700000000006</v>
+      </c>
+      <c r="C63">
+        <v>10.32066</v>
+      </c>
+      <c r="D63">
+        <v>0.93030000000000002</v>
+      </c>
+      <c r="E63">
+        <v>0.37940000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64">
+        <v>-0.13039000000000001</v>
+      </c>
+      <c r="C64">
+        <v>0.16675000000000001</v>
+      </c>
+      <c r="D64">
+        <v>-0.78200000000000003</v>
+      </c>
+      <c r="E64">
+        <v>0.45669999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66">
+        <v>0.1043719</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67">
+        <v>0.46614</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68">
+        <v>0.64344000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A36:F37"/>
+    <mergeCell ref="A1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52094E53-0DB4-EA4C-BBCB-536ACA6FB929}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1.5202637999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.2636791</v>
+      </c>
+      <c r="D10">
+        <v>5.7656000000000001</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8.9419999999999994E-5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11">
+        <v>7.5905E-3</v>
+      </c>
+      <c r="C11">
+        <v>3.0863000000000002E-3</v>
+      </c>
+      <c r="D11">
+        <v>2.4594</v>
+      </c>
+      <c r="E11">
+        <v>3.007E-2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>-0.80111960000000004</v>
+      </c>
+      <c r="C12">
+        <v>0.27870709999999999</v>
+      </c>
+      <c r="D12">
+        <v>-2.8744000000000001</v>
+      </c>
+      <c r="E12">
+        <v>1.397E-2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>0.59910079999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>8.9663599999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>4.15E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DFC9F1-EA15-944A-AFAD-8EC1EC1D1B61}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>4.3948635600000001</v>
+      </c>
+      <c r="C10">
+        <v>27.74295673</v>
+      </c>
+      <c r="D10">
+        <v>0.15840000000000001</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.87860000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>-0.19519585</v>
+      </c>
+      <c r="C11">
+        <v>0.59359287999999999</v>
+      </c>
+      <c r="D11">
+        <v>-0.32879999999999998</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0.75190000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>6.8177391399999996</v>
+      </c>
+      <c r="C12">
+        <v>12.13136068</v>
+      </c>
+      <c r="D12">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0.5917</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13">
+        <v>1.4465999999999999E-4</v>
+      </c>
+      <c r="C13">
+        <v>9.0552000000000004E-4</v>
+      </c>
+      <c r="D13">
+        <v>0.1598</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.87760000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>0.1173638</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>0.31025999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>0.81764999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>-1846.1079999999999</v>
+      </c>
+      <c r="C29">
+        <v>10272.915000000001</v>
+      </c>
+      <c r="D29">
+        <v>-0.1797</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.86250000000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>637.60699999999997</v>
+      </c>
+      <c r="C30">
+        <v>67.257999999999996</v>
+      </c>
+      <c r="D30">
+        <v>9.48</v>
+      </c>
+      <c r="E30" s="3">
+        <v>3.0389999999999999E-5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>-2224.2359999999999</v>
+      </c>
+      <c r="C31">
+        <v>5289.7120000000004</v>
+      </c>
+      <c r="D31">
+        <v>-0.42049999999999998</v>
+      </c>
+      <c r="E31">
+        <v>0.68669999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>1624.2570000000001</v>
+      </c>
+      <c r="C32">
+        <v>7202.7929999999997</v>
+      </c>
+      <c r="D32">
+        <v>0.22550000000000001</v>
+      </c>
+      <c r="E32">
+        <v>0.82799999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>0.78321470000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>1.0070000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82104B4-1C31-834F-AD98-04B252774FF6}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0.30863069999999998</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.2530673</v>
+      </c>
+      <c r="D2" s="12">
+        <v>3.972</v>
+      </c>
+      <c r="E2" s="8">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8">
+        <v>36</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1.3766910000000001</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1.2351447</v>
+      </c>
+      <c r="D3" s="12">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8">
+        <v>15</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1.4708954000000001</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1.2153881</v>
+      </c>
+      <c r="D4" s="12">
+        <v>7.7859999999999996</v>
+      </c>
+      <c r="E4" s="8">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="12">
+        <v>2.0524388999999998</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1.4750763</v>
+      </c>
+      <c r="D5" s="12">
+        <v>10.143000000000001</v>
+      </c>
+      <c r="E5" s="8">
+        <v>5</v>
+      </c>
+      <c r="F5" s="8">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2.1996574999999998</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1.9730038000000001</v>
+      </c>
+      <c r="D6" s="12">
+        <v>29.538</v>
+      </c>
+      <c r="E6" s="8">
+        <v>12</v>
+      </c>
+      <c r="F6" s="8">
+        <v>39</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="12">
+        <v>2.2714219999999998</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2.0762347999999999</v>
+      </c>
+      <c r="D7" s="12">
+        <v>37.01</v>
+      </c>
+      <c r="E7" s="8">
+        <v>13</v>
+      </c>
+      <c r="F7" s="8">
+        <v>50</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2.8887421999999998</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2.7790499</v>
+      </c>
+      <c r="D8" s="12">
+        <v>184.36500000000001</v>
+      </c>
+      <c r="E8" s="8">
+        <v>77</v>
+      </c>
+      <c r="F8" s="8">
+        <v>564</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>43</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8">
+        <v>2</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>3</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0.46023439999999999</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.34883209999999998</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>2</v>
+      </c>
+      <c r="F14" s="8">
+        <v>9</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.81718369999999996</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.56233509999999998</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>2</v>
+      </c>
+      <c r="F15" s="8">
+        <v>4</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.73432529999999996</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.66156320000000002</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2</v>
+      </c>
+      <c r="F16" s="8">
+        <v>8</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.70253969999999999</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.50040240000000002</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8">
+        <v>2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>5</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="12">
+        <v>0.74977519999999998</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.68696159999999995</v>
+      </c>
+      <c r="D18" s="12">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2</v>
+      </c>
+      <c r="F18" s="8">
+        <v>9</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="12">
+        <v>0.98534630000000001</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.63651420000000003</v>
+      </c>
+      <c r="D19" s="12">
+        <v>2.3330000000000002</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2</v>
+      </c>
+      <c r="F19" s="8">
+        <v>3</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="12">
+        <v>1.8184534999999999</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1.566608</v>
+      </c>
+      <c r="D20" s="12">
+        <v>15.019</v>
+      </c>
+      <c r="E20" s="8">
+        <v>9</v>
+      </c>
+      <c r="F20" s="8">
+        <v>27</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="12">
+        <v>0.53520939999999995</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0.46402070000000001</v>
+      </c>
+      <c r="D21" s="12">
+        <v>41.735999999999997</v>
+      </c>
+      <c r="E21" s="8">
+        <v>10</v>
+      </c>
+      <c r="F21" s="8">
+        <v>121</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="12">
+        <v>1.3862943999999999</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0.69314719999999996</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="8">
+        <v>2</v>
+      </c>
+      <c r="F22" s="8">
+        <v>2</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8">
+        <v>1</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1.3862943999999999</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0.69314719999999996</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="8">
+        <v>2</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26" s="8">
+        <v>1</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="12">
+        <v>0</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1</v>
+      </c>
+      <c r="F27" s="8">
+        <v>1</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="12">
+        <v>0</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1</v>
+      </c>
+      <c r="F28" s="8">
+        <v>35</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="8"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H28">
+    <sortCondition ref="G3:G28"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>